<commit_message>
update utils.py exclude bug
</commit_message>
<xml_diff>
--- a/forager-cochlear/data/lexical_data/foods/corrections.xlsx
+++ b/forager-cochlear/data/lexical_data/foods/corrections.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhilashakumar/Documents/active projects/forager_project/cochlear-full/forager-cochlear/data/lexical_data/foods/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854211E7-9C18-4140-A0C6-8355D5F4B93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAEBC73F-1CFA-5044-843C-A76038F6DAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{D764696C-5266-A44C-BF6C-11D44431CF68}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="308">
   <si>
     <t>milk</t>
   </si>
@@ -594,12 +594,6 @@
   </si>
   <si>
     <t>beverage</t>
-  </si>
-  <si>
-    <t>langus</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>lasagna</t>
@@ -1357,20 +1351,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C8A1EED-9F2B-BE4C-82C7-2BB11A533FF5}">
-  <dimension ref="A1:B235"/>
+  <dimension ref="A1:B234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2426,12 +2420,12 @@
         <v>188</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>189</v>
+        <v>111</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>111</v>
@@ -2439,26 +2433,26 @@
     </row>
     <row r="135" spans="1:2">
       <c r="A135" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>111</v>
+        <v>21</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B137" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="B137" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2466,15 +2460,15 @@
         <v>194</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B139" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="B139" s="3" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2482,12 +2476,12 @@
         <v>197</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>198</v>
+        <v>152</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>152</v>
@@ -2495,34 +2489,34 @@
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>152</v>
+        <v>45</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>6</v>
+        <v>96</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B145" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="B145" s="3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2538,47 +2532,47 @@
         <v>206</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>207</v>
+        <v>133</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>133</v>
+        <v>21</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>0</v>
+        <v>72</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B152" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -2586,15 +2580,15 @@
         <v>213</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>214</v>
+        <v>111</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B154" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="B154" s="3" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -2602,31 +2596,31 @@
         <v>216</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>217</v>
+        <v>65</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B158" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="B158" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -2634,44 +2628,44 @@
         <v>221</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>222</v>
+        <v>84</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>108</v>
+        <v>4</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B164" s="3" t="s">
         <v>72</v>
@@ -2679,26 +2673,26 @@
     </row>
     <row r="165" spans="1:2">
       <c r="A165" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>72</v>
+        <v>6</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B167" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="B167" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -2706,31 +2700,31 @@
         <v>231</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>232</v>
+        <v>62</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>96</v>
+        <v>13</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B171" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="B171" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -2738,55 +2732,55 @@
         <v>236</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>237</v>
+        <v>105</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>105</v>
+        <v>136</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>147</v>
+        <v>68</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B178" s="3" t="s">
         <v>243</v>
-      </c>
-      <c r="B178" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -2794,36 +2788,36 @@
         <v>244</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>245</v>
+        <v>62</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B183" s="3" t="s">
         <v>42</v>
@@ -2831,58 +2825,58 @@
     </row>
     <row r="184" spans="1:2">
       <c r="A184" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>42</v>
+        <v>111</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>126</v>
+        <v>17</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>45</v>
+        <v>140</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>140</v>
+        <v>62</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B190" s="3" t="s">
         <v>256</v>
-      </c>
-      <c r="B190" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -2890,15 +2884,15 @@
         <v>257</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>258</v>
+        <v>23</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B192" s="3" t="s">
         <v>259</v>
-      </c>
-      <c r="B192" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -2906,23 +2900,23 @@
         <v>260</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>261</v>
+        <v>160</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>160</v>
+        <v>256</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B195" s="3" t="s">
         <v>263</v>
-      </c>
-      <c r="B195" s="3" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -2930,60 +2924,60 @@
         <v>264</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>265</v>
+        <v>108</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>68</v>
+        <v>215</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>217</v>
+        <v>72</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>49</v>
+        <v>185</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B203" s="3" t="s">
         <v>185</v>
@@ -2991,7 +2985,7 @@
     </row>
     <row r="204" spans="1:2">
       <c r="A204" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B204" s="3" t="s">
         <v>185</v>
@@ -2999,114 +2993,114 @@
     </row>
     <row r="205" spans="1:2">
       <c r="A205" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>185</v>
+        <v>72</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>72</v>
+        <v>115</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>115</v>
+        <v>23</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>47</v>
+        <v>140</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>152</v>
+        <v>111</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>111</v>
+        <v>0</v>
       </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>0</v>
+        <v>72</v>
       </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>72</v>
+        <v>136</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>136</v>
+        <v>176</v>
       </c>
     </row>
     <row r="217" spans="1:2">
       <c r="A217" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>176</v>
+        <v>42</v>
       </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B218" s="3" t="s">
         <v>287</v>
-      </c>
-      <c r="B218" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="219" spans="1:2">
@@ -3114,15 +3108,15 @@
         <v>288</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>289</v>
+        <v>136</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B220" s="3" t="s">
         <v>290</v>
-      </c>
-      <c r="B220" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -3130,15 +3124,15 @@
         <v>291</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>292</v>
+        <v>80</v>
       </c>
     </row>
     <row r="222" spans="1:2">
       <c r="A222" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B222" s="3" t="s">
         <v>293</v>
-      </c>
-      <c r="B222" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="223" spans="1:2">
@@ -3146,20 +3140,20 @@
         <v>294</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>295</v>
+        <v>111</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B225" s="3" t="s">
         <v>111</v>
@@ -3167,39 +3161,39 @@
     </row>
     <row r="226" spans="1:2">
       <c r="A226" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>111</v>
+        <v>45</v>
       </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B230" s="3" t="s">
         <v>124</v>
@@ -3207,41 +3201,33 @@
     </row>
     <row r="231" spans="1:2">
       <c r="A231" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>124</v>
+        <v>8</v>
       </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="233" spans="1:2">
       <c r="A233" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>0</v>
+        <v>115</v>
       </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2">
-      <c r="A235" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="B235" s="3" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
corrected typos in corrections file
</commit_message>
<xml_diff>
--- a/forager-cochlear/data/lexical_data/foods/corrections.xlsx
+++ b/forager-cochlear/data/lexical_data/foods/corrections.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bowdoin-my.sharepoint.com/personal/c_hambric_bowdoin_edu/Documents/Documents/cochlear-full/forager-cochlear/data/lexical_data/foods/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\forager-cochlear\data\lexical_data\foods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{AAEBC73F-1CFA-5044-843C-A76038F6DAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA4693B8-7BD1-4B19-AB3F-34C4B5EEBD6B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26DEB651-847F-4801-8AE4-CF5C2053BEC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D764696C-5266-A44C-BF6C-11D44431CF68}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D764696C-5266-A44C-BF6C-11D44431CF68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="306">
   <si>
     <t>milk</t>
   </si>
@@ -269,9 +269,6 @@
     <t>chickennoodlesoup</t>
   </si>
   <si>
-    <t>souo</t>
-  </si>
-  <si>
     <t>chickennuggets</t>
   </si>
   <si>
@@ -533,9 +530,6 @@
     <t>hashbrowns</t>
   </si>
   <si>
-    <t>potatloes</t>
-  </si>
-  <si>
     <t>hershey</t>
   </si>
   <si>
@@ -645,9 +639,6 @@
   </si>
   <si>
     <t>mashedpotatoes</t>
-  </si>
-  <si>
-    <t>potoes</t>
   </si>
   <si>
     <t>mayo</t>
@@ -1356,18 +1347,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C8A1EED-9F2B-BE4C-82C7-2BB11A533FF5}">
   <dimension ref="A1:B235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="E238" sqref="E238"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1727,12 +1718,12 @@
         <v>76</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>38</v>
@@ -1740,15 +1731,15 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>23</v>
@@ -1756,7 +1747,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>4</v>
@@ -1764,15 +1755,15 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>38</v>
@@ -1780,7 +1771,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>38</v>
@@ -1788,15 +1779,15 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>45</v>
@@ -1804,47 +1795,47 @@
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>0</v>
@@ -1852,7 +1843,7 @@
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>4</v>
@@ -1860,23 +1851,23 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>70</v>
@@ -1884,7 +1875,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>4</v>
@@ -1892,7 +1883,7 @@
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>4</v>
@@ -1900,15 +1891,15 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>15</v>
@@ -1916,15 +1907,15 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>65</v>
@@ -1932,23 +1923,23 @@
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>6</v>
@@ -1956,23 +1947,23 @@
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>70</v>
@@ -1980,7 +1971,7 @@
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>72</v>
@@ -1988,23 +1979,23 @@
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B79" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>72</v>
@@ -2012,23 +2003,23 @@
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B83" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>72</v>
@@ -2036,7 +2027,7 @@
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>72</v>
@@ -2044,7 +2035,7 @@
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>72</v>
@@ -2052,7 +2043,7 @@
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>72</v>
@@ -2060,7 +2051,7 @@
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>72</v>
@@ -2068,15 +2059,15 @@
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B89" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>23</v>
@@ -2084,39 +2075,39 @@
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B91" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B92" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B93" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>4</v>
@@ -2124,15 +2115,15 @@
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>62</v>
@@ -2140,7 +2131,7 @@
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>15</v>
@@ -2148,15 +2139,15 @@
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B99" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>72</v>
@@ -2164,7 +2155,7 @@
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>68</v>
@@ -2172,7 +2163,7 @@
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>8</v>
@@ -2180,31 +2171,31 @@
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B103" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>6</v>
@@ -2212,7 +2203,7 @@
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>25</v>
@@ -2220,7 +2211,7 @@
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>17</v>
@@ -2228,7 +2219,7 @@
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>17</v>
@@ -2236,31 +2227,31 @@
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B111" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>40</v>
@@ -2268,7 +2259,7 @@
     </row>
     <row r="114" spans="1:2">
       <c r="A114" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>40</v>
@@ -2276,55 +2267,55 @@
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>15</v>
@@ -2332,7 +2323,7 @@
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>38</v>
@@ -2340,103 +2331,103 @@
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>21</v>
@@ -2444,7 +2435,7 @@
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>49</v>
@@ -2452,47 +2443,47 @@
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>45</v>
@@ -2500,7 +2491,7 @@
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>6</v>
@@ -2508,39 +2499,39 @@
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>203</v>
+        <v>135</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>21</v>
@@ -2548,7 +2539,7 @@
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B149" s="3" t="s">
         <v>0</v>
@@ -2556,7 +2547,7 @@
     </row>
     <row r="150" spans="1:2">
       <c r="A150" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B150" s="3" t="s">
         <v>72</v>
@@ -2564,7 +2555,7 @@
     </row>
     <row r="151" spans="1:2">
       <c r="A151" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B151" s="3" t="s">
         <v>45</v>
@@ -2572,31 +2563,31 @@
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B155" s="3" t="s">
         <v>65</v>
@@ -2604,7 +2595,7 @@
     </row>
     <row r="156" spans="1:2">
       <c r="A156" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B156" s="3" t="s">
         <v>23</v>
@@ -2612,7 +2603,7 @@
     </row>
     <row r="157" spans="1:2">
       <c r="A157" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B157" s="3" t="s">
         <v>6</v>
@@ -2620,23 +2611,23 @@
     </row>
     <row r="158" spans="1:2">
       <c r="A158" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B160" s="3" t="s">
         <v>65</v>
@@ -2644,15 +2635,15 @@
     </row>
     <row r="161" spans="1:2">
       <c r="A161" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B162" s="3" t="s">
         <v>4</v>
@@ -2660,7 +2651,7 @@
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B163" s="3" t="s">
         <v>72</v>
@@ -2668,7 +2659,7 @@
     </row>
     <row r="164" spans="1:2">
       <c r="A164" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B164" s="3" t="s">
         <v>72</v>
@@ -2676,7 +2667,7 @@
     </row>
     <row r="165" spans="1:2">
       <c r="A165" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B165" s="3" t="s">
         <v>6</v>
@@ -2684,7 +2675,7 @@
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B166" s="3" t="s">
         <v>4</v>
@@ -2692,15 +2683,15 @@
     </row>
     <row r="167" spans="1:2">
       <c r="A167" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B168" s="3" t="s">
         <v>62</v>
@@ -2708,15 +2699,15 @@
     </row>
     <row r="169" spans="1:2">
       <c r="A169" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B170" s="3" t="s">
         <v>13</v>
@@ -2724,47 +2715,47 @@
     </row>
     <row r="171" spans="1:2">
       <c r="A171" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B176" s="3" t="s">
         <v>68</v>
@@ -2772,23 +2763,23 @@
     </row>
     <row r="177" spans="1:2">
       <c r="A177" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B179" s="3" t="s">
         <v>62</v>
@@ -2796,7 +2787,7 @@
     </row>
     <row r="180" spans="1:2">
       <c r="A180" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B180" s="3" t="s">
         <v>4</v>
@@ -2804,7 +2795,7 @@
     </row>
     <row r="181" spans="1:2">
       <c r="A181" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B181" s="3" t="s">
         <v>62</v>
@@ -2812,7 +2803,7 @@
     </row>
     <row r="182" spans="1:2">
       <c r="A182" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B182" s="3" t="s">
         <v>42</v>
@@ -2820,7 +2811,7 @@
     </row>
     <row r="183" spans="1:2">
       <c r="A183" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B183" s="3" t="s">
         <v>42</v>
@@ -2828,23 +2819,23 @@
     </row>
     <row r="184" spans="1:2">
       <c r="A184" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B186" s="3" t="s">
         <v>17</v>
@@ -2852,7 +2843,7 @@
     </row>
     <row r="187" spans="1:2">
       <c r="A187" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B187" s="3" t="s">
         <v>45</v>
@@ -2860,15 +2851,15 @@
     </row>
     <row r="188" spans="1:2">
       <c r="A188" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B189" s="3" t="s">
         <v>62</v>
@@ -2876,15 +2867,15 @@
     </row>
     <row r="190" spans="1:2">
       <c r="A190" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B191" s="3" t="s">
         <v>23</v>
@@ -2892,47 +2883,47 @@
     </row>
     <row r="192" spans="1:2">
       <c r="A192" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B197" s="3" t="s">
         <v>68</v>
@@ -2940,15 +2931,15 @@
     </row>
     <row r="198" spans="1:2">
       <c r="A198" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B199" s="3" t="s">
         <v>72</v>
@@ -2956,7 +2947,7 @@
     </row>
     <row r="200" spans="1:2">
       <c r="A200" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B200" s="3" t="s">
         <v>0</v>
@@ -2964,7 +2955,7 @@
     </row>
     <row r="201" spans="1:2">
       <c r="A201" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B201" s="3" t="s">
         <v>49</v>
@@ -2972,31 +2963,31 @@
     </row>
     <row r="202" spans="1:2">
       <c r="A202" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B205" s="3" t="s">
         <v>72</v>
@@ -3004,15 +2995,15 @@
     </row>
     <row r="206" spans="1:2">
       <c r="A206" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B207" s="3" t="s">
         <v>23</v>
@@ -3020,7 +3011,7 @@
     </row>
     <row r="208" spans="1:2">
       <c r="A208" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B208" s="3" t="s">
         <v>72</v>
@@ -3028,7 +3019,7 @@
     </row>
     <row r="209" spans="1:2">
       <c r="A209" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B209" s="3" t="s">
         <v>47</v>
@@ -3036,31 +3027,31 @@
     </row>
     <row r="210" spans="1:2">
       <c r="A210" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B213" s="3" t="s">
         <v>0</v>
@@ -3068,7 +3059,7 @@
     </row>
     <row r="214" spans="1:2">
       <c r="A214" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B214" s="3" t="s">
         <v>72</v>
@@ -3076,23 +3067,23 @@
     </row>
     <row r="215" spans="1:2">
       <c r="A215" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="217" spans="1:2">
       <c r="A217" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B217" s="3" t="s">
         <v>42</v>
@@ -3100,71 +3091,71 @@
     </row>
     <row r="218" spans="1:2">
       <c r="A218" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="219" spans="1:2">
       <c r="A219" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="221" spans="1:2">
       <c r="A221" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="222" spans="1:2">
       <c r="A222" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="223" spans="1:2">
       <c r="A223" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B226" s="3" t="s">
         <v>45</v>
@@ -3172,7 +3163,7 @@
     </row>
     <row r="227" spans="1:2">
       <c r="A227" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B227" s="3" t="s">
         <v>70</v>
@@ -3180,31 +3171,31 @@
     </row>
     <row r="228" spans="1:2">
       <c r="A228" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="231" spans="1:2">
       <c r="A231" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B231" s="3" t="s">
         <v>8</v>
@@ -3212,7 +3203,7 @@
     </row>
     <row r="232" spans="1:2">
       <c r="A232" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B232" s="3" t="s">
         <v>0</v>
@@ -3220,15 +3211,15 @@
     </row>
     <row r="233" spans="1:2">
       <c r="A233" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B234" s="3" t="s">
         <v>15</v>
@@ -3236,10 +3227,10 @@
     </row>
     <row r="235" spans="1:2">
       <c r="A235" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>